<commit_message>
Set decimal precision in Aermod input same as HEM3
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jill Mozier\OneDrive - SC&amp;A, Inc\Projects\RIS-409 to 104 RTR  NATA (2013-2017)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="E3A1ED2A2AB344E4A436B3918830E2EED1C541F9" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7E16BE87-DDF4-4D91-AB98-DBC8BDE74279}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="E3A1ED2A2AB344E4A436B3918830E2EED1C541F9" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{A54BF85A-E0FA-4066-B701-7A37C87217CB}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="150" windowWidth="25905" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
ej implemented for multiple combos...still need to use risk thresholds and infer toshis
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BFA6F-4D68-4608-B1D1-9B839808A064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B6AAB8-86E4-46C9-A9EE-836A873E3D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="528" yWindow="792" windowWidth="22380" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,7 +1464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A312" sqref="A312:XFD312"/>
+      <selection pane="bottomLeft" activeCell="A311" sqref="A311:XFD311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated target organ file
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scainccloud-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B6AAB8-86E4-46C9-A9EE-836A873E3D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="E3A1ED2A2AB344E4A436B3918830E2EED1C541F9" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E69A0938-2FE9-464A-9B1B-48284C276DCD}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="792" windowWidth="22380" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="1380" windowWidth="19500" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target Organ Endpoints" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="326">
   <si>
     <t>pollutant</t>
   </si>
@@ -1002,33 +1002,6 @@
   </si>
   <si>
     <t>1,2,3,4,6,7,8,9-Octachlorodibenzofuran</t>
-  </si>
-  <si>
-    <t>uranium hexafluoride</t>
-  </si>
-  <si>
-    <t>uranium (iv) dioxide</t>
-  </si>
-  <si>
-    <t>uranyl acetate dihydrate</t>
-  </si>
-  <si>
-    <t>uranium, soluble</t>
-  </si>
-  <si>
-    <t>uranium oxide</t>
-  </si>
-  <si>
-    <t>uranium, insoluble</t>
-  </si>
-  <si>
-    <t>triethylene glycol monohexyl ether</t>
-  </si>
-  <si>
-    <t>uranyl nitrate hexahydrate</t>
-  </si>
-  <si>
-    <t>isopropyl cyanide</t>
   </si>
 </sst>
 </file>
@@ -1460,34 +1433,34 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P312"/>
+  <dimension ref="A1:P303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A311" sqref="A311:XFD311"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="2"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>245</v>
       </c>
@@ -1587,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1637,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1687,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>324</v>
       </c>
@@ -1737,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>325</v>
       </c>
@@ -1787,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1837,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
@@ -1887,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>308</v>
       </c>
@@ -1937,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1987,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>309</v>
       </c>
@@ -2037,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2087,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>310</v>
       </c>
@@ -2137,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -2187,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>311</v>
       </c>
@@ -2237,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2287,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>312</v>
       </c>
@@ -2337,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2387,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -2437,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -2487,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -2537,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -2587,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -2637,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -2687,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -2737,7 +2710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>313</v>
       </c>
@@ -2787,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>314</v>
       </c>
@@ -2837,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2887,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>315</v>
       </c>
@@ -2937,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -2987,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3037,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -3087,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3137,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3187,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3237,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3287,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>319</v>
       </c>
@@ -3337,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -3387,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
@@ -3437,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3487,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>242</v>
       </c>
@@ -3537,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -3587,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -3637,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -3687,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -3737,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -3787,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -3837,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -3887,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -3937,7 +3910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>56</v>
       </c>
@@ -3987,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -4037,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
@@ -4087,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -4137,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>255</v>
       </c>
@@ -4184,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>256</v>
       </c>
@@ -4231,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>257</v>
       </c>
@@ -4278,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>258</v>
       </c>
@@ -4325,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>259</v>
       </c>
@@ -4372,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -4422,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -4472,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -4522,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>260</v>
       </c>
@@ -4569,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -4619,7 +4592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -4669,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -4719,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -4769,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -4819,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -4869,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>268</v>
       </c>
@@ -4916,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -4966,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -5016,7 +4989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>322</v>
       </c>
@@ -5063,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>261</v>
       </c>
@@ -5110,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
@@ -5160,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>262</v>
       </c>
@@ -5207,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>263</v>
       </c>
@@ -5254,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
@@ -5304,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>73</v>
       </c>
@@ -5354,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>74</v>
       </c>
@@ -5404,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>75</v>
       </c>
@@ -5454,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>76</v>
       </c>
@@ -5504,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>77</v>
       </c>
@@ -5554,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>318</v>
       </c>
@@ -5601,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>78</v>
       </c>
@@ -5651,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
@@ -5701,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>264</v>
       </c>
@@ -5748,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>80</v>
       </c>
@@ -5798,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>270</v>
       </c>
@@ -5845,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -5892,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
         <v>246</v>
       </c>
@@ -5942,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>81</v>
       </c>
@@ -5992,7 +5965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>82</v>
       </c>
@@ -6042,7 +6015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>306</v>
       </c>
@@ -6089,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>83</v>
       </c>
@@ -6139,7 +6112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>84</v>
       </c>
@@ -6189,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>85</v>
       </c>
@@ -6239,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
@@ -6289,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>87</v>
       </c>
@@ -6339,7 +6312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>235</v>
       </c>
@@ -6389,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>88</v>
       </c>
@@ -6439,7 +6412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>89</v>
       </c>
@@ -6489,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>90</v>
       </c>
@@ -6539,7 +6512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>91</v>
       </c>
@@ -6589,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>92</v>
       </c>
@@ -6639,7 +6612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>93</v>
       </c>
@@ -6689,7 +6662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>291</v>
       </c>
@@ -6736,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>94</v>
       </c>
@@ -6786,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>265</v>
       </c>
@@ -6833,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>95</v>
       </c>
@@ -6883,7 +6856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>266</v>
       </c>
@@ -6930,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>96</v>
       </c>
@@ -6980,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
@@ -7030,7 +7003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
@@ -7080,7 +7053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
@@ -7130,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>267</v>
       </c>
@@ -7177,7 +7150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>100</v>
       </c>
@@ -7227,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>303</v>
       </c>
@@ -7277,7 +7250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>236</v>
       </c>
@@ -7327,7 +7300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>101</v>
       </c>
@@ -7377,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>102</v>
       </c>
@@ -7427,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>271</v>
       </c>
@@ -7474,7 +7447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>103</v>
       </c>
@@ -7524,7 +7497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
         <v>317</v>
       </c>
@@ -7571,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>272</v>
       </c>
@@ -7618,7 +7591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>273</v>
       </c>
@@ -7665,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>274</v>
       </c>
@@ -7712,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>275</v>
       </c>
@@ -7759,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>276</v>
       </c>
@@ -7806,7 +7779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>277</v>
       </c>
@@ -7853,7 +7826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>104</v>
       </c>
@@ -7903,7 +7876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>105</v>
       </c>
@@ -7953,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>106</v>
       </c>
@@ -8003,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>107</v>
       </c>
@@ -8053,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>108</v>
       </c>
@@ -8103,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>247</v>
       </c>
@@ -8153,7 +8126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>109</v>
       </c>
@@ -8203,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>110</v>
       </c>
@@ -8253,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>111</v>
       </c>
@@ -8303,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>112</v>
       </c>
@@ -8353,7 +8326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>113</v>
       </c>
@@ -8403,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>305</v>
       </c>
@@ -8450,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>114</v>
       </c>
@@ -8500,7 +8473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>115</v>
       </c>
@@ -8550,7 +8523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>244</v>
       </c>
@@ -8600,7 +8573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>116</v>
       </c>
@@ -8650,7 +8623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>117</v>
       </c>
@@ -8700,7 +8673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>278</v>
       </c>
@@ -8747,7 +8720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>118</v>
       </c>
@@ -8797,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>119</v>
       </c>
@@ -8847,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>120</v>
       </c>
@@ -8897,7 +8870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>321</v>
       </c>
@@ -8947,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>121</v>
       </c>
@@ -8997,7 +8970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>122</v>
       </c>
@@ -9047,7 +9020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>123</v>
       </c>
@@ -9097,7 +9070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>124</v>
       </c>
@@ -9147,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>125</v>
       </c>
@@ -9197,7 +9170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>126</v>
       </c>
@@ -9247,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>127</v>
       </c>
@@ -9297,7 +9270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>248</v>
       </c>
@@ -9347,7 +9320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>128</v>
       </c>
@@ -9397,7 +9370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>129</v>
       </c>
@@ -9447,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>130</v>
       </c>
@@ -9497,7 +9470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>131</v>
       </c>
@@ -9547,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>249</v>
       </c>
@@ -9597,7 +9570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>132</v>
       </c>
@@ -9647,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>133</v>
       </c>
@@ -9697,7 +9670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>134</v>
       </c>
@@ -9747,7 +9720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>135</v>
       </c>
@@ -9797,7 +9770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>137</v>
       </c>
@@ -9847,7 +9820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>138</v>
       </c>
@@ -9897,7 +9870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>139</v>
       </c>
@@ -9947,7 +9920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>140</v>
       </c>
@@ -9997,7 +9970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>141</v>
       </c>
@@ -10047,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>142</v>
       </c>
@@ -10097,7 +10070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>143</v>
       </c>
@@ -10147,7 +10120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>144</v>
       </c>
@@ -10197,7 +10170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>145</v>
       </c>
@@ -10247,7 +10220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>237</v>
       </c>
@@ -10297,7 +10270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>146</v>
       </c>
@@ -10347,7 +10320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>147</v>
       </c>
@@ -10361,10 +10334,10 @@
         <v>0</v>
       </c>
       <c r="E180" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F180" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G180" s="2">
         <v>0</v>
@@ -10397,7 +10370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>148</v>
       </c>
@@ -10411,10 +10384,10 @@
         <v>0</v>
       </c>
       <c r="E181" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F181" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G181" s="2">
         <v>0</v>
@@ -10447,7 +10420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>149</v>
       </c>
@@ -10461,10 +10434,10 @@
         <v>0</v>
       </c>
       <c r="E182" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F182" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G182" s="2">
         <v>0</v>
@@ -10497,7 +10470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>150</v>
       </c>
@@ -10511,10 +10484,10 @@
         <v>0</v>
       </c>
       <c r="E183" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F183" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G183" s="2">
         <v>0</v>
@@ -10547,7 +10520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>151</v>
       </c>
@@ -10561,10 +10534,10 @@
         <v>0</v>
       </c>
       <c r="E184" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F184" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G184" s="2">
         <v>0</v>
@@ -10597,7 +10570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>286</v>
       </c>
@@ -10608,10 +10581,10 @@
         <v>0</v>
       </c>
       <c r="E185" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F185" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G185" s="2">
         <v>0</v>
@@ -10644,7 +10617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>152</v>
       </c>
@@ -10658,10 +10631,10 @@
         <v>0</v>
       </c>
       <c r="E186" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F186" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G186" s="2">
         <v>0</v>
@@ -10694,7 +10667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>243</v>
       </c>
@@ -10708,10 +10681,10 @@
         <v>0</v>
       </c>
       <c r="E187" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F187" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G187" s="2">
         <v>0</v>
@@ -10744,7 +10717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>153</v>
       </c>
@@ -10758,10 +10731,10 @@
         <v>0</v>
       </c>
       <c r="E188" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F188" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G188" s="2">
         <v>0</v>
@@ -10794,7 +10767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>154</v>
       </c>
@@ -10808,10 +10781,10 @@
         <v>0</v>
       </c>
       <c r="E189" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F189" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G189" s="2">
         <v>0</v>
@@ -10844,7 +10817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>155</v>
       </c>
@@ -10858,10 +10831,10 @@
         <v>0</v>
       </c>
       <c r="E190" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F190" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G190" s="2">
         <v>0</v>
@@ -10894,7 +10867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>156</v>
       </c>
@@ -10908,10 +10881,10 @@
         <v>0</v>
       </c>
       <c r="E191" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F191" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G191" s="2">
         <v>0</v>
@@ -10944,7 +10917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>157</v>
       </c>
@@ -10994,7 +10967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>158</v>
       </c>
@@ -11044,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>289</v>
       </c>
@@ -11091,7 +11064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>159</v>
       </c>
@@ -11141,7 +11114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>160</v>
       </c>
@@ -11191,7 +11164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>241</v>
       </c>
@@ -11241,7 +11214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>290</v>
       </c>
@@ -11288,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>161</v>
       </c>
@@ -11338,7 +11311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>162</v>
       </c>
@@ -11388,7 +11361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>323</v>
       </c>
@@ -11438,7 +11411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>163</v>
       </c>
@@ -11488,7 +11461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>233</v>
       </c>
@@ -11538,7 +11511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>250</v>
       </c>
@@ -11588,7 +11561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>164</v>
       </c>
@@ -11638,7 +11611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>251</v>
       </c>
@@ -11688,7 +11661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>252</v>
       </c>
@@ -11738,7 +11711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>165</v>
       </c>
@@ -11788,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>292</v>
       </c>
@@ -11835,7 +11808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>166</v>
       </c>
@@ -11885,7 +11858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>167</v>
       </c>
@@ -11935,7 +11908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>285</v>
       </c>
@@ -11982,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>293</v>
       </c>
@@ -12029,7 +12002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>168</v>
       </c>
@@ -12079,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>169</v>
       </c>
@@ -12129,7 +12102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>316</v>
       </c>
@@ -12176,7 +12149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>170</v>
       </c>
@@ -12226,7 +12199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>171</v>
       </c>
@@ -12276,7 +12249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>172</v>
       </c>
@@ -12326,7 +12299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>173</v>
       </c>
@@ -12376,7 +12349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>294</v>
       </c>
@@ -12423,7 +12396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>174</v>
       </c>
@@ -12473,7 +12446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>175</v>
       </c>
@@ -12523,7 +12496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>176</v>
       </c>
@@ -12573,7 +12546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>177</v>
       </c>
@@ -12623,7 +12596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>295</v>
       </c>
@@ -12670,7 +12643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -12720,7 +12693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>178</v>
       </c>
@@ -12770,7 +12743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>179</v>
       </c>
@@ -12820,7 +12793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>180</v>
       </c>
@@ -12870,7 +12843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>181</v>
       </c>
@@ -12920,7 +12893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>182</v>
       </c>
@@ -12970,7 +12943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>297</v>
       </c>
@@ -13017,7 +12990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>183</v>
       </c>
@@ -13067,7 +13040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>184</v>
       </c>
@@ -13117,7 +13090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>185</v>
       </c>
@@ -13167,7 +13140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>186</v>
       </c>
@@ -13217,7 +13190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
         <v>187</v>
       </c>
@@ -13267,7 +13240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>188</v>
       </c>
@@ -13317,7 +13290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>189</v>
       </c>
@@ -13367,7 +13340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>190</v>
       </c>
@@ -13417,7 +13390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>234</v>
       </c>
@@ -13467,7 +13440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>231</v>
       </c>
@@ -13517,7 +13490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>253</v>
       </c>
@@ -13567,7 +13540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>238</v>
       </c>
@@ -13617,7 +13590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
         <v>191</v>
       </c>
@@ -13667,7 +13640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
         <v>192</v>
       </c>
@@ -13717,7 +13690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
         <v>193</v>
       </c>
@@ -13767,7 +13740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>194</v>
       </c>
@@ -13817,7 +13790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>296</v>
       </c>
@@ -13864,7 +13837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
         <v>195</v>
       </c>
@@ -13914,7 +13887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
         <v>196</v>
       </c>
@@ -13964,7 +13937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>197</v>
       </c>
@@ -14014,7 +13987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
         <v>198</v>
       </c>
@@ -14064,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>279</v>
       </c>
@@ -14111,7 +14084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
         <v>199</v>
       </c>
@@ -14161,7 +14134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
         <v>298</v>
       </c>
@@ -14208,7 +14181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
         <v>280</v>
       </c>
@@ -14255,7 +14228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>281</v>
       </c>
@@ -14302,7 +14275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
         <v>254</v>
       </c>
@@ -14349,7 +14322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
         <v>200</v>
       </c>
@@ -14399,7 +14372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
         <v>201</v>
       </c>
@@ -14449,7 +14422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>202</v>
       </c>
@@ -14499,7 +14472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>232</v>
       </c>
@@ -14549,7 +14522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
         <v>299</v>
       </c>
@@ -14596,7 +14569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
         <v>203</v>
       </c>
@@ -14646,7 +14619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
         <v>204</v>
       </c>
@@ -14696,7 +14669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
         <v>205</v>
       </c>
@@ -14746,7 +14719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
         <v>206</v>
       </c>
@@ -14796,7 +14769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
         <v>239</v>
       </c>
@@ -14846,7 +14819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
         <v>207</v>
       </c>
@@ -14896,7 +14869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
         <v>208</v>
       </c>
@@ -14946,7 +14919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
         <v>300</v>
       </c>
@@ -14993,7 +14966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
         <v>282</v>
       </c>
@@ -15040,7 +15013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>209</v>
       </c>
@@ -15090,7 +15063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
         <v>283</v>
       </c>
@@ -15137,7 +15110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>210</v>
       </c>
@@ -15187,7 +15160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
         <v>301</v>
       </c>
@@ -15234,7 +15207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
         <v>302</v>
       </c>
@@ -15281,7 +15254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
         <v>211</v>
       </c>
@@ -15331,7 +15304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
         <v>212</v>
       </c>
@@ -15381,7 +15354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>213</v>
       </c>
@@ -15431,7 +15404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>214</v>
       </c>
@@ -15481,7 +15454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
         <v>287</v>
       </c>
@@ -15528,7 +15501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>288</v>
       </c>
@@ -15575,7 +15548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>304</v>
       </c>
@@ -15622,7 +15595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
         <v>284</v>
       </c>
@@ -15669,7 +15642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A288" s="2" t="s">
         <v>216</v>
       </c>
@@ -15719,7 +15692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
         <v>217</v>
       </c>
@@ -15769,7 +15742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290" s="2" t="s">
         <v>218</v>
       </c>
@@ -15819,7 +15792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
         <v>219</v>
       </c>
@@ -15869,7 +15842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292" s="6" t="s">
         <v>320</v>
       </c>
@@ -15919,7 +15892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293" s="2" t="s">
         <v>220</v>
       </c>
@@ -15969,7 +15942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294" s="2" t="s">
         <v>221</v>
       </c>
@@ -16019,7 +15992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295" s="2" t="s">
         <v>222</v>
       </c>
@@ -16069,7 +16042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296" s="2" t="s">
         <v>223</v>
       </c>
@@ -16119,7 +16092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
         <v>224</v>
       </c>
@@ -16169,7 +16142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298" s="2" t="s">
         <v>225</v>
       </c>
@@ -16219,7 +16192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
         <v>226</v>
       </c>
@@ -16269,7 +16242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" s="2" t="s">
         <v>227</v>
       </c>
@@ -16319,7 +16292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301" s="2" t="s">
         <v>228</v>
       </c>
@@ -16369,7 +16342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302" s="2" t="s">
         <v>240</v>
       </c>
@@ -16419,7 +16392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303" s="2" t="s">
         <v>229</v>
       </c>
@@ -16467,51 +16440,6 @@
       </c>
       <c r="P303" s="2">
         <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A304" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -16520,7 +16448,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RNovember 1, 2017</oddFooter>
+    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RApril 8, 2021</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed word demographic to community; check for run group folder in dash app
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scainccloud-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="E3A1ED2A2AB344E4A436B3918830E2EED1C541F9" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E69A0938-2FE9-464A-9B1B-48284C276DCD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA6ABDC-BD59-4F39-BFC1-00E0DB47D313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="1380" windowWidth="19500" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target Organ Endpoints" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="335">
   <si>
     <t>pollutant</t>
   </si>
@@ -1002,6 +1002,33 @@
   </si>
   <si>
     <t>1,2,3,4,6,7,8,9-Octachlorodibenzofuran</t>
+  </si>
+  <si>
+    <t>uranium hexafluoride</t>
+  </si>
+  <si>
+    <t>uranium (iv) dioxide</t>
+  </si>
+  <si>
+    <t>uranyl acetate dihydrate</t>
+  </si>
+  <si>
+    <t>uranium, soluble</t>
+  </si>
+  <si>
+    <t>uranium oxide</t>
+  </si>
+  <si>
+    <t>uranium, insoluble</t>
+  </si>
+  <si>
+    <t>triethylene glycol monohexyl ether</t>
+  </si>
+  <si>
+    <t>uranyl nitrate hexahydrate</t>
+  </si>
+  <si>
+    <t>isopropyl cyanide</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1091,6 +1118,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1433,34 +1461,34 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P303"/>
+  <dimension ref="A1:P312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
+      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>245</v>
       </c>
@@ -1560,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>324</v>
       </c>
@@ -1710,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>325</v>
       </c>
@@ -1760,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1810,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
@@ -1860,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>308</v>
       </c>
@@ -1910,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1960,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>309</v>
       </c>
@@ -2010,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2060,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>310</v>
       </c>
@@ -2110,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -2160,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>311</v>
       </c>
@@ -2210,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2260,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>312</v>
       </c>
@@ -2310,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2360,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -2410,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -2460,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -2510,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -2560,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -2610,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -2660,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>313</v>
       </c>
@@ -2760,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>314</v>
       </c>
@@ -2810,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2860,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>315</v>
       </c>
@@ -2910,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -2960,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3010,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -3060,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3110,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3160,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3210,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3260,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>319</v>
       </c>
@@ -3310,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -3360,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
@@ -3410,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3460,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>242</v>
       </c>
@@ -3510,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -3560,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -3610,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -3660,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -3710,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -3760,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -3810,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -3860,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -3910,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>56</v>
       </c>
@@ -3960,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -4010,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
@@ -4060,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -4110,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>255</v>
       </c>
@@ -4157,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>256</v>
       </c>
@@ -4204,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>257</v>
       </c>
@@ -4251,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>258</v>
       </c>
@@ -4298,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>259</v>
       </c>
@@ -4345,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -4395,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -4445,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -4495,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>260</v>
       </c>
@@ -4542,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -4592,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -4642,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -4692,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -4742,7 +4770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -4792,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -4842,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>268</v>
       </c>
@@ -4889,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -4939,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -4989,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>322</v>
       </c>
@@ -5036,7 +5064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>261</v>
       </c>
@@ -5083,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
@@ -5133,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>262</v>
       </c>
@@ -5180,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>263</v>
       </c>
@@ -5227,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
@@ -5277,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>73</v>
       </c>
@@ -5327,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>74</v>
       </c>
@@ -5377,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>75</v>
       </c>
@@ -5427,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>76</v>
       </c>
@@ -5477,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>77</v>
       </c>
@@ -5527,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>318</v>
       </c>
@@ -5574,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>78</v>
       </c>
@@ -5624,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
@@ -5674,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>264</v>
       </c>
@@ -5721,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>80</v>
       </c>
@@ -5771,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>270</v>
       </c>
@@ -5818,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -5865,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>246</v>
       </c>
@@ -5915,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>81</v>
       </c>
@@ -5965,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>82</v>
       </c>
@@ -6015,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>306</v>
       </c>
@@ -6062,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>83</v>
       </c>
@@ -6112,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>84</v>
       </c>
@@ -6162,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>85</v>
       </c>
@@ -6212,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
@@ -6262,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>87</v>
       </c>
@@ -6312,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>235</v>
       </c>
@@ -6362,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>88</v>
       </c>
@@ -6412,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>89</v>
       </c>
@@ -6462,7 +6490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>90</v>
       </c>
@@ -6512,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>91</v>
       </c>
@@ -6562,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>92</v>
       </c>
@@ -6612,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>93</v>
       </c>
@@ -6662,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>291</v>
       </c>
@@ -6709,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>94</v>
       </c>
@@ -6759,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>265</v>
       </c>
@@ -6806,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>95</v>
       </c>
@@ -6856,7 +6884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>266</v>
       </c>
@@ -6903,7 +6931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>96</v>
       </c>
@@ -6953,7 +6981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
@@ -7003,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
@@ -7053,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
@@ -7103,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>267</v>
       </c>
@@ -7150,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>100</v>
       </c>
@@ -7200,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>303</v>
       </c>
@@ -7250,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>236</v>
       </c>
@@ -7300,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>101</v>
       </c>
@@ -7350,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>102</v>
       </c>
@@ -7400,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>271</v>
       </c>
@@ -7447,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>103</v>
       </c>
@@ -7497,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>317</v>
       </c>
@@ -7544,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>272</v>
       </c>
@@ -7591,7 +7619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>273</v>
       </c>
@@ -7638,7 +7666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>274</v>
       </c>
@@ -7685,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>275</v>
       </c>
@@ -7732,7 +7760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>276</v>
       </c>
@@ -7779,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>277</v>
       </c>
@@ -7826,7 +7854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>104</v>
       </c>
@@ -7876,7 +7904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>105</v>
       </c>
@@ -7926,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>106</v>
       </c>
@@ -7976,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>107</v>
       </c>
@@ -8026,7 +8054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>108</v>
       </c>
@@ -8076,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>247</v>
       </c>
@@ -8126,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>109</v>
       </c>
@@ -8176,7 +8204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>110</v>
       </c>
@@ -8226,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>111</v>
       </c>
@@ -8276,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>112</v>
       </c>
@@ -8326,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>113</v>
       </c>
@@ -8376,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>305</v>
       </c>
@@ -8423,7 +8451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>114</v>
       </c>
@@ -8473,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>115</v>
       </c>
@@ -8523,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>244</v>
       </c>
@@ -8573,7 +8601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>116</v>
       </c>
@@ -8623,7 +8651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>117</v>
       </c>
@@ -8673,7 +8701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>278</v>
       </c>
@@ -8720,7 +8748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>118</v>
       </c>
@@ -8770,7 +8798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>119</v>
       </c>
@@ -8820,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>120</v>
       </c>
@@ -8870,7 +8898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>321</v>
       </c>
@@ -8920,7 +8948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>121</v>
       </c>
@@ -8970,7 +8998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>122</v>
       </c>
@@ -9020,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>123</v>
       </c>
@@ -9070,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>124</v>
       </c>
@@ -9120,7 +9148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>125</v>
       </c>
@@ -9170,7 +9198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>126</v>
       </c>
@@ -9220,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>127</v>
       </c>
@@ -9270,7 +9298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>248</v>
       </c>
@@ -9320,7 +9348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>128</v>
       </c>
@@ -9370,7 +9398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>129</v>
       </c>
@@ -9420,7 +9448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>130</v>
       </c>
@@ -9470,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>131</v>
       </c>
@@ -9520,7 +9548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>249</v>
       </c>
@@ -9570,7 +9598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>132</v>
       </c>
@@ -9620,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>133</v>
       </c>
@@ -9670,7 +9698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>134</v>
       </c>
@@ -9720,7 +9748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>135</v>
       </c>
@@ -9770,7 +9798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>137</v>
       </c>
@@ -9820,7 +9848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>138</v>
       </c>
@@ -9870,7 +9898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>139</v>
       </c>
@@ -9920,7 +9948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>140</v>
       </c>
@@ -9970,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>141</v>
       </c>
@@ -10020,7 +10048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>142</v>
       </c>
@@ -10070,7 +10098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>143</v>
       </c>
@@ -10120,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>144</v>
       </c>
@@ -10170,7 +10198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>145</v>
       </c>
@@ -10220,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>237</v>
       </c>
@@ -10270,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>146</v>
       </c>
@@ -10320,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>147</v>
       </c>
@@ -10370,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>148</v>
       </c>
@@ -10420,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>149</v>
       </c>
@@ -10470,7 +10498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>150</v>
       </c>
@@ -10520,7 +10548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>151</v>
       </c>
@@ -10570,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>286</v>
       </c>
@@ -10617,7 +10645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>152</v>
       </c>
@@ -10667,7 +10695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>243</v>
       </c>
@@ -10717,7 +10745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>153</v>
       </c>
@@ -10767,7 +10795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>154</v>
       </c>
@@ -10817,7 +10845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>155</v>
       </c>
@@ -10867,7 +10895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>156</v>
       </c>
@@ -10917,7 +10945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>157</v>
       </c>
@@ -10967,7 +10995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>158</v>
       </c>
@@ -11017,7 +11045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>289</v>
       </c>
@@ -11064,7 +11092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>159</v>
       </c>
@@ -11114,7 +11142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>160</v>
       </c>
@@ -11164,7 +11192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>241</v>
       </c>
@@ -11214,7 +11242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>290</v>
       </c>
@@ -11261,7 +11289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>161</v>
       </c>
@@ -11311,7 +11339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>162</v>
       </c>
@@ -11361,7 +11389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>323</v>
       </c>
@@ -11411,7 +11439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>163</v>
       </c>
@@ -11461,7 +11489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>233</v>
       </c>
@@ -11511,7 +11539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>250</v>
       </c>
@@ -11561,7 +11589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>164</v>
       </c>
@@ -11611,7 +11639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>251</v>
       </c>
@@ -11661,7 +11689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>252</v>
       </c>
@@ -11711,7 +11739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>165</v>
       </c>
@@ -11761,7 +11789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>292</v>
       </c>
@@ -11808,7 +11836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>166</v>
       </c>
@@ -11858,7 +11886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>167</v>
       </c>
@@ -11908,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>285</v>
       </c>
@@ -11955,7 +11983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>293</v>
       </c>
@@ -12002,7 +12030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>168</v>
       </c>
@@ -12052,7 +12080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>169</v>
       </c>
@@ -12102,7 +12130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>316</v>
       </c>
@@ -12149,7 +12177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>170</v>
       </c>
@@ -12199,7 +12227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>171</v>
       </c>
@@ -12249,7 +12277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>172</v>
       </c>
@@ -12299,7 +12327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>173</v>
       </c>
@@ -12349,7 +12377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>294</v>
       </c>
@@ -12396,7 +12424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>174</v>
       </c>
@@ -12446,7 +12474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>175</v>
       </c>
@@ -12496,7 +12524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>176</v>
       </c>
@@ -12546,7 +12574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>177</v>
       </c>
@@ -12596,7 +12624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>295</v>
       </c>
@@ -12643,7 +12671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -12693,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>178</v>
       </c>
@@ -12743,7 +12771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>179</v>
       </c>
@@ -12793,7 +12821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>180</v>
       </c>
@@ -12843,7 +12871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>181</v>
       </c>
@@ -12893,7 +12921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>182</v>
       </c>
@@ -12943,7 +12971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>297</v>
       </c>
@@ -12990,7 +13018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>183</v>
       </c>
@@ -13040,7 +13068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>184</v>
       </c>
@@ -13090,7 +13118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>185</v>
       </c>
@@ -13140,7 +13168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>186</v>
       </c>
@@ -13190,7 +13218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>187</v>
       </c>
@@ -13240,7 +13268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>188</v>
       </c>
@@ -13290,7 +13318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>189</v>
       </c>
@@ -13340,7 +13368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>190</v>
       </c>
@@ -13390,7 +13418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>234</v>
       </c>
@@ -13440,7 +13468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>231</v>
       </c>
@@ -13490,7 +13518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>253</v>
       </c>
@@ -13540,7 +13568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>238</v>
       </c>
@@ -13590,7 +13618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>191</v>
       </c>
@@ -13640,7 +13668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>192</v>
       </c>
@@ -13690,7 +13718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>193</v>
       </c>
@@ -13740,7 +13768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>194</v>
       </c>
@@ -13790,7 +13818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>296</v>
       </c>
@@ -13837,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>195</v>
       </c>
@@ -13887,7 +13915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>196</v>
       </c>
@@ -13937,7 +13965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>197</v>
       </c>
@@ -13987,7 +14015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>198</v>
       </c>
@@ -14037,7 +14065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>279</v>
       </c>
@@ -14084,7 +14112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>199</v>
       </c>
@@ -14134,7 +14162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>298</v>
       </c>
@@ -14181,7 +14209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>280</v>
       </c>
@@ -14228,7 +14256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>281</v>
       </c>
@@ -14275,7 +14303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>254</v>
       </c>
@@ -14322,7 +14350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>200</v>
       </c>
@@ -14372,7 +14400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>201</v>
       </c>
@@ -14422,7 +14450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>202</v>
       </c>
@@ -14472,7 +14500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>232</v>
       </c>
@@ -14522,7 +14550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>299</v>
       </c>
@@ -14569,7 +14597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>203</v>
       </c>
@@ -14619,7 +14647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>204</v>
       </c>
@@ -14669,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>205</v>
       </c>
@@ -14719,7 +14747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>206</v>
       </c>
@@ -14769,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>239</v>
       </c>
@@ -14819,7 +14847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>207</v>
       </c>
@@ -14869,7 +14897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>208</v>
       </c>
@@ -14919,7 +14947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>300</v>
       </c>
@@ -14966,7 +14994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>282</v>
       </c>
@@ -15013,7 +15041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>209</v>
       </c>
@@ -15063,7 +15091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>283</v>
       </c>
@@ -15110,7 +15138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>210</v>
       </c>
@@ -15160,7 +15188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>301</v>
       </c>
@@ -15207,7 +15235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>302</v>
       </c>
@@ -15254,7 +15282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>211</v>
       </c>
@@ -15304,7 +15332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>212</v>
       </c>
@@ -15354,7 +15382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>213</v>
       </c>
@@ -15404,7 +15432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>214</v>
       </c>
@@ -15454,7 +15482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>287</v>
       </c>
@@ -15501,7 +15529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>288</v>
       </c>
@@ -15548,7 +15576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>304</v>
       </c>
@@ -15595,7 +15623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>284</v>
       </c>
@@ -15642,7 +15670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>216</v>
       </c>
@@ -15692,7 +15720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>217</v>
       </c>
@@ -15742,7 +15770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>218</v>
       </c>
@@ -15792,7 +15820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>219</v>
       </c>
@@ -15842,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>320</v>
       </c>
@@ -15892,7 +15920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>220</v>
       </c>
@@ -15942,7 +15970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>221</v>
       </c>
@@ -15992,7 +16020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>222</v>
       </c>
@@ -16042,7 +16070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>223</v>
       </c>
@@ -16092,7 +16120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>224</v>
       </c>
@@ -16142,7 +16170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>225</v>
       </c>
@@ -16192,7 +16220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>226</v>
       </c>
@@ -16242,7 +16270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>227</v>
       </c>
@@ -16292,7 +16320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>228</v>
       </c>
@@ -16342,7 +16370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>240</v>
       </c>
@@ -16392,7 +16420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>229</v>
       </c>
@@ -16440,6 +16468,51 @@
       </c>
       <c r="P303" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A304" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="9" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="9" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="9" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled NoHS demo in ejdash, fixed bug in MultiPathway, new dose response tables
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scainccloud-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{4CA6ABDC-BD59-4F39-BFC1-00E0DB47D313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0A9429A-1497-4376-A80C-54ACB12C8C8D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{187F83E8-D374-488D-8A28-123AE97F1433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="315" windowWidth="18885" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="1575" windowWidth="20220" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target Organ Endpoints" sheetId="1" r:id="rId1"/>
@@ -1464,8 +1464,8 @@
   <dimension ref="A1:P312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8618,13 +8618,13 @@
         <v>0</v>
       </c>
       <c r="F145" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G145" s="2">
         <v>0</v>
       </c>
       <c r="H145" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145" s="2">
         <v>0</v>
@@ -13626,10 +13626,10 @@
         <v>19</v>
       </c>
       <c r="C246" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D246" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E246" s="2">
         <v>0</v>
@@ -16899,7 +16899,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RApril 21, 2021</oddFooter>
+    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RJune 9, 2021</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New users guide, updated dose response, fix to altrec inner to handle C/P/V
</commit_message>
<xml_diff>
--- a/resources/Target_Organ_Endpoints.xlsx
+++ b/resources/Target_Organ_Endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scainccloud-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/hollingsworth_terri_epa_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{187F83E8-D374-488D-8A28-123AE97F1433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{6FDEEBF1-2654-4809-85E9-8CD92A92ACE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4C3E9F76-EB6F-40A8-9098-114678022949}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="1575" windowWidth="20220" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target Organ Endpoints" sheetId="1" r:id="rId1"/>
@@ -1464,31 +1464,31 @@
   <dimension ref="A1:P312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A246" sqref="A246"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>245</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -1688,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>324</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>325</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>308</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>309</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>310</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>311</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>312</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>313</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>314</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>315</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -2999,10 +2999,10 @@
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>319</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>242</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
@@ -3858,10 +3858,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -3888,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>56</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>255</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>256</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>257</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>258</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>259</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>260</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>268</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -4978,10 +4978,10 @@
         <v>0</v>
       </c>
       <c r="D71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="2">
         <v>0</v>
@@ -5017,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>322</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>261</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>262</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>263</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>73</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>0</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -5325,10 +5325,10 @@
         <v>0</v>
       </c>
       <c r="G78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" s="2">
         <v>0</v>
@@ -5355,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>74</v>
       </c>
@@ -5363,10 +5363,10 @@
         <v>20</v>
       </c>
       <c r="C79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -5405,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>75</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>76</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>77</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>318</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>78</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>264</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>80</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>270</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>246</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>81</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>82</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>306</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>83</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>84</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>85</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>87</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>235</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>88</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>89</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>90</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>91</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>92</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>93</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>291</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>94</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>265</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>95</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>266</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>96</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>267</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>100</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>303</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>236</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>101</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>102</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>271</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>103</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>317</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>272</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>273</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>274</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>275</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>276</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>277</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>104</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>105</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>106</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>107</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>108</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>247</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>109</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>110</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>111</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>112</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>113</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>305</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>114</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>115</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>244</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>116</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>117</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>278</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>118</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>119</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>120</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>321</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>121</v>
       </c>
@@ -8998,7 +8998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>122</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>123</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>124</v>
       </c>
@@ -9148,7 +9148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>125</v>
       </c>
@@ -9198,7 +9198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>126</v>
       </c>
@@ -9248,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>127</v>
       </c>
@@ -9298,7 +9298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>248</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>128</v>
       </c>
@@ -9398,7 +9398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>129</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="J161" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" s="2">
         <v>0</v>
@@ -9448,7 +9448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>130</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>131</v>
       </c>
@@ -9548,7 +9548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>249</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>132</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>133</v>
       </c>
@@ -9659,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="D166" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E166" s="2">
         <v>0</v>
@@ -9698,7 +9698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>134</v>
       </c>
@@ -9718,7 +9718,7 @@
         <v>0</v>
       </c>
       <c r="G167" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H167" s="2">
         <v>0</v>
@@ -9748,7 +9748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>135</v>
       </c>
@@ -9798,7 +9798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>137</v>
       </c>
@@ -9848,7 +9848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>138</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>139</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>140</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>141</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>142</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>143</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>144</v>
       </c>
@@ -10198,7 +10198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>145</v>
       </c>
@@ -10209,10 +10209,10 @@
         <v>0</v>
       </c>
       <c r="D177" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E177" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F177" s="2">
         <v>0</v>
@@ -10230,7 +10230,7 @@
         <v>0</v>
       </c>
       <c r="K177" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L177" s="2">
         <v>0</v>
@@ -10248,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>237</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>146</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>147</v>
       </c>
@@ -10398,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>148</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>149</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>150</v>
       </c>
@@ -10548,7 +10548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>151</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>286</v>
       </c>
@@ -10645,7 +10645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>152</v>
       </c>
@@ -10695,7 +10695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>243</v>
       </c>
@@ -10745,7 +10745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>153</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>154</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>155</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>156</v>
       </c>
@@ -10945,7 +10945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>157</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>0</v>
       </c>
       <c r="D192" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E192" s="2">
         <v>0</v>
@@ -10965,10 +10965,10 @@
         <v>0</v>
       </c>
       <c r="G192" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H192" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I192" s="2">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>158</v>
       </c>
@@ -11045,7 +11045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>289</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>159</v>
       </c>
@@ -11142,7 +11142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>160</v>
       </c>
@@ -11192,7 +11192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>241</v>
       </c>
@@ -11242,7 +11242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>290</v>
       </c>
@@ -11289,7 +11289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>161</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>162</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>323</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>163</v>
       </c>
@@ -11489,7 +11489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>233</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>250</v>
       </c>
@@ -11589,7 +11589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>164</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>251</v>
       </c>
@@ -11689,7 +11689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>252</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>165</v>
       </c>
@@ -11789,7 +11789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>292</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>166</v>
       </c>
@@ -11886,7 +11886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>167</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>285</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>293</v>
       </c>
@@ -12030,7 +12030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>168</v>
       </c>
@@ -12080,7 +12080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>169</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>316</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>170</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>171</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>172</v>
       </c>
@@ -12327,7 +12327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>173</v>
       </c>
@@ -12377,7 +12377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>294</v>
       </c>
@@ -12424,7 +12424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>174</v>
       </c>
@@ -12474,7 +12474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>175</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>176</v>
       </c>
@@ -12574,7 +12574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>177</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>295</v>
       </c>
@@ -12671,7 +12671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>178</v>
       </c>
@@ -12771,7 +12771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>179</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>180</v>
       </c>
@@ -12871,7 +12871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>181</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>182</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>297</v>
       </c>
@@ -13018,7 +13018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>183</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>184</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>185</v>
       </c>
@@ -13168,7 +13168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>186</v>
       </c>
@@ -13218,7 +13218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>187</v>
       </c>
@@ -13268,7 +13268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>188</v>
       </c>
@@ -13318,7 +13318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>189</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>190</v>
       </c>
@@ -13418,7 +13418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>234</v>
       </c>
@@ -13468,7 +13468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>231</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>253</v>
       </c>
@@ -13568,7 +13568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>238</v>
       </c>
@@ -13618,7 +13618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>191</v>
       </c>
@@ -13668,7 +13668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>192</v>
       </c>
@@ -13679,7 +13679,7 @@
         <v>0</v>
       </c>
       <c r="D247" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E247" s="2">
         <v>0</v>
@@ -13691,7 +13691,7 @@
         <v>0</v>
       </c>
       <c r="H247" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I247" s="2">
         <v>0</v>
@@ -13718,7 +13718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>193</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>194</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>296</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>195</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>196</v>
       </c>
@@ -13965,7 +13965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>197</v>
       </c>
@@ -14015,7 +14015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>198</v>
       </c>
@@ -14065,7 +14065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>279</v>
       </c>
@@ -14112,7 +14112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>199</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>298</v>
       </c>
@@ -14209,7 +14209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>280</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>281</v>
       </c>
@@ -14303,7 +14303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>254</v>
       </c>
@@ -14350,7 +14350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>200</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>201</v>
       </c>
@@ -14450,7 +14450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>202</v>
       </c>
@@ -14500,7 +14500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>232</v>
       </c>
@@ -14550,7 +14550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>299</v>
       </c>
@@ -14597,7 +14597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>203</v>
       </c>
@@ -14647,7 +14647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>204</v>
       </c>
@@ -14697,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>205</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>206</v>
       </c>
@@ -14797,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>239</v>
       </c>
@@ -14847,7 +14847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>207</v>
       </c>
@@ -14897,7 +14897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>208</v>
       </c>
@@ -14947,7 +14947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>300</v>
       </c>
@@ -14994,7 +14994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>282</v>
       </c>
@@ -15041,7 +15041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>209</v>
       </c>
@@ -15091,7 +15091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>283</v>
       </c>
@@ -15138,7 +15138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>210</v>
       </c>
@@ -15188,7 +15188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>301</v>
       </c>
@@ -15235,7 +15235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>302</v>
       </c>
@@ -15282,7 +15282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>211</v>
       </c>
@@ -15332,7 +15332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>212</v>
       </c>
@@ -15382,7 +15382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>213</v>
       </c>
@@ -15390,7 +15390,7 @@
         <v>29</v>
       </c>
       <c r="C282" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D282" s="2">
         <v>0</v>
@@ -15432,7 +15432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>214</v>
       </c>
@@ -15482,7 +15482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>287</v>
       </c>
@@ -15529,7 +15529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>288</v>
       </c>
@@ -15576,7 +15576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>304</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>284</v>
       </c>
@@ -15670,7 +15670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>216</v>
       </c>
@@ -15720,7 +15720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>217</v>
       </c>
@@ -15770,7 +15770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>218</v>
       </c>
@@ -15820,7 +15820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>219</v>
       </c>
@@ -15870,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>320</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>220</v>
       </c>
@@ -15970,7 +15970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>221</v>
       </c>
@@ -16020,7 +16020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>222</v>
       </c>
@@ -16070,7 +16070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>223</v>
       </c>
@@ -16120,7 +16120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>224</v>
       </c>
@@ -16170,7 +16170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>225</v>
       </c>
@@ -16220,7 +16220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>226</v>
       </c>
@@ -16270,7 +16270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>227</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>228</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>240</v>
       </c>
@@ -16420,7 +16420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>229</v>
       </c>
@@ -16470,7 +16470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304" s="9" t="s">
         <v>326</v>
       </c>
@@ -16517,7 +16517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A305" s="9" t="s">
         <v>327</v>
       </c>
@@ -16564,7 +16564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A306" s="9" t="s">
         <v>328</v>
       </c>
@@ -16611,7 +16611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A307" s="9" t="s">
         <v>329</v>
       </c>
@@ -16658,7 +16658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A308" s="9" t="s">
         <v>330</v>
       </c>
@@ -16705,7 +16705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A309" s="9" t="s">
         <v>331</v>
       </c>
@@ -16752,7 +16752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A310" s="9" t="s">
         <v>332</v>
       </c>
@@ -16799,7 +16799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A311" s="9" t="s">
         <v>333</v>
       </c>
@@ -16846,7 +16846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A312" s="9" t="s">
         <v>334</v>
       </c>
@@ -16899,7 +16899,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RJune 9, 2021</oddFooter>
+    <oddFooter>&amp;LTarget Organ Endpoints&amp;C&amp;P&amp;RAugust 31, 2021</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>